<commit_message>
Lab03 - white box testing
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243D7E68-2167-469E-976F-3AC1910B9C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A092F2C0-452F-4708-9A7B-5553C89846AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="326" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" tabRatio="326" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
     <sheet name="F01.ECP" sheetId="2" r:id="rId2"/>
-    <sheet name="BBT-TCs" sheetId="4" r:id="rId3"/>
-    <sheet name="F01.BVA" sheetId="3" r:id="rId4"/>
+    <sheet name="F01.BVA" sheetId="3" r:id="rId3"/>
+    <sheet name="BBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,6 +34,41 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+max = 
+Current Year</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
@@ -68,43 +103,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-max = 
-Current Year</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="97">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -351,9 +351,6 @@
     <t>TC4_BVA</t>
   </si>
   <si>
-    <t>TC5_BVA</t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -522,18 +519,12 @@
     </r>
   </si>
   <si>
-    <t>02. table= 2</t>
-  </si>
-  <si>
     <t>03. table = 0</t>
   </si>
   <si>
     <t>04. table = 1</t>
   </si>
   <si>
-    <t>01. table = 7</t>
-  </si>
-  <si>
     <t>amount: double &gt; 0.0</t>
   </si>
   <si>
@@ -549,21 +540,9 @@
     <t>06. amount = 0.01</t>
   </si>
   <si>
-    <t>07. amount = 50</t>
-  </si>
-  <si>
-    <t>05. table = -1</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
-    <t>01, 06</t>
-  </si>
-  <si>
-    <t>02, 07</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -573,25 +552,19 @@
     <t>08. amount = 0</t>
   </si>
   <si>
-    <t>09. amount = -0.01</t>
-  </si>
-  <si>
-    <t>05, 09</t>
-  </si>
-  <si>
     <t>04, 08</t>
   </si>
   <si>
-    <t>-0.01</t>
-  </si>
-  <si>
     <t>TC2_ECP</t>
   </si>
   <si>
-    <t>TC2_BVA</t>
-  </si>
-  <si>
     <t>TC1_BVA</t>
+  </si>
+  <si>
+    <t>02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01. </t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1216,6 +1189,48 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1231,10 +1246,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1258,29 +1294,104 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1293,147 +1404,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1744,8 +1714,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1759,12 +1729,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
       <c r="H1" s="25" t="s">
         <v>1</v>
       </c>
@@ -1772,11 +1742,11 @@
       <c r="J1" s="25"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.45">
       <c r="H3" s="2"/>
@@ -1792,7 +1762,7 @@
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J4" s="2">
         <v>235</v>
@@ -1803,7 +1773,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -1857,8 +1827,8 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="B15" s="71" t="s">
-        <v>68</v>
+      <c r="B15" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1866,7 +1836,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1889,7 +1859,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="21"/>
     </row>
@@ -1934,21 +1904,21 @@
     </row>
     <row r="24" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="22"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C26" s="24"/>
@@ -1971,7 +1941,7 @@
   </sheetPr>
   <dimension ref="B1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1991,38 +1961,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B3" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="G5" s="37" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="G5" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" s="9" t="s">
@@ -2037,59 +2007,59 @@
       <c r="E6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="46"/>
-      <c r="K6" s="42" t="s">
+      <c r="J6" s="52"/>
+      <c r="K6" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="43"/>
+      <c r="L6" s="51"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>71</v>
+      <c r="C7" s="53" t="s">
+        <v>70</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="43"/>
+      <c r="L7" s="51"/>
     </row>
     <row r="8" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="2">
         <v>1</v>
@@ -2097,27 +2067,27 @@
       <c r="J8" s="2">
         <v>100</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="41"/>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>72</v>
+      <c r="C9" s="53" t="s">
+        <v>71</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="9">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" s="2">
         <v>0</v>
@@ -2125,25 +2095,25 @@
       <c r="J9" s="2">
         <v>100</v>
       </c>
-      <c r="K9" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="L9" s="41"/>
+      <c r="K9" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="31"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="72">
+        <v>86</v>
+      </c>
+      <c r="G10" s="27">
         <v>3</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="12">
         <v>1</v>
@@ -2151,10 +2121,10 @@
       <c r="J10" s="12">
         <v>-50</v>
       </c>
-      <c r="K10" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="57"/>
+      <c r="K10" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="62"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
@@ -2163,19 +2133,12 @@
     </row>
     <row r="12" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K7:L7"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
@@ -2184,450 +2147,27 @@
     <mergeCell ref="G5:L5"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor theme="7" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="B1:K21"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B3" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B4" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="81" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="81"/>
-    </row>
-    <row r="5" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="82"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="86" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="86" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="86" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="87">
-        <v>1</v>
-      </c>
-      <c r="C6" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="89" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="92">
-        <v>1</v>
-      </c>
-      <c r="G6" s="92">
-        <v>100</v>
-      </c>
-      <c r="H6" s="92" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="87" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B7" s="72">
-        <f>B6+1</f>
-        <v>2</v>
-      </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="93">
-        <v>0</v>
-      </c>
-      <c r="G7" s="93">
-        <v>100</v>
-      </c>
-      <c r="H7" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B8" s="72">
-        <f t="shared" ref="B8:B13" si="0">B7+1</f>
-        <v>3</v>
-      </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="90" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="93">
-        <v>1</v>
-      </c>
-      <c r="G8" s="93">
-        <v>-50</v>
-      </c>
-      <c r="H8" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B9" s="72">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="88"/>
-      <c r="D9" s="97" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="94">
-        <v>7</v>
-      </c>
-      <c r="G9" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="H9" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="72" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B10" s="72">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="93">
-        <v>2</v>
-      </c>
-      <c r="G10" s="93">
-        <v>50</v>
-      </c>
-      <c r="H10" s="93" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="72" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B11" s="72">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="93">
-        <v>0</v>
-      </c>
-      <c r="G11" s="93" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B12" s="72">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="93">
-        <v>1</v>
-      </c>
-      <c r="G12" s="93">
-        <v>0</v>
-      </c>
-      <c r="H12" s="93" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="86">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="91"/>
-      <c r="D13" s="98" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="95">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="95" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" s="86" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="2:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="C17" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="67"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="66"/>
-    </row>
-    <row r="18" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="69" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B19" s="60"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="63"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B20" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="14">
-        <v>8</v>
-      </c>
-      <c r="D20" s="16">
-        <v>8</v>
-      </c>
-      <c r="E20" s="16">
-        <v>0</v>
-      </c>
-      <c r="F20" s="17">
-        <v>0</v>
-      </c>
-      <c r="G20" s="20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="16">
-        <v>8</v>
-      </c>
-      <c r="K20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="H21" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:I3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N15"/>
+  <dimension ref="B1:N14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2647,40 +2187,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B3" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="6" spans="2:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="4" t="s">
@@ -2693,257 +2233,610 @@
         <v>33</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="L6" s="58"/>
-      <c r="M6" s="54" t="s">
+      <c r="L6" s="89"/>
+      <c r="M6" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="55"/>
+      <c r="N6" s="92"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B7" s="32">
+      <c r="B7" s="93">
         <v>1</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>87</v>
+      <c r="C7" s="95" t="s">
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="45"/>
+        <v>96</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" s="42" t="s">
+      <c r="M7" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="43"/>
+      <c r="N7" s="51"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B8" s="48"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="J8" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K8" s="12">
         <v>7</v>
       </c>
-      <c r="L8" s="73" t="s">
-        <v>93</v>
-      </c>
-      <c r="M8" s="56" t="s">
+      <c r="L8" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M8" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="57"/>
+      <c r="N8" s="62"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B9" s="48"/>
-      <c r="C9" s="50"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="72">
-        <v>2</v>
+        <v>81</v>
+      </c>
+      <c r="G9" s="9">
+        <v>3</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="73">
-        <v>2</v>
-      </c>
-      <c r="L9" s="73">
-        <v>50</v>
-      </c>
-      <c r="M9" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="57"/>
+        <v>41</v>
+      </c>
+      <c r="K9" s="28">
+        <v>0</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="62"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B10" s="48"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G10" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="73">
+      <c r="K10" s="28">
+        <v>1</v>
+      </c>
+      <c r="L10" s="28">
         <v>0</v>
       </c>
-      <c r="L10" s="73" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="N10" s="57"/>
+      <c r="M10" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="62"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B11" s="48"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="93">
+        <v>3</v>
+      </c>
+      <c r="C11" s="95" t="s">
+        <v>83</v>
+      </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="9">
-        <v>4</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="73">
-        <v>1</v>
-      </c>
-      <c r="L11" s="73">
-        <v>0</v>
-      </c>
-      <c r="M11" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="N11" s="57"/>
+        <v>87</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B12" s="32">
-        <v>3</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="72">
-        <v>5</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="73">
-        <v>-1</v>
-      </c>
-      <c r="L12" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="M12" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="N12" s="57"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B13" s="48"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B14" s="48"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B15" s="48"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:L14"/>
+  <mergeCells count="21">
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="G5:N5"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:L12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="B1:K21"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B3" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B4" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="82"/>
+      <c r="H4" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="80"/>
+    </row>
+    <row r="5" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="74"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="30">
+        <v>1</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>100</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B7" s="27">
+        <f>B6+1</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="34">
+        <v>0</v>
+      </c>
+      <c r="G7" s="34">
+        <v>100</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B8" s="27">
+        <f t="shared" ref="B8:B13" si="0">B7+1</f>
+        <v>3</v>
+      </c>
+      <c r="C8" s="71"/>
+      <c r="D8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="34">
+        <v>1</v>
+      </c>
+      <c r="G8" s="34">
+        <v>-50</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B9" s="27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="71"/>
+      <c r="D9" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="35">
+        <v>7</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B10" s="27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B11" s="27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="71"/>
+      <c r="D11" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="34">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B12" s="27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="71"/>
+      <c r="D12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="34">
+        <v>1</v>
+      </c>
+      <c r="G12" s="34">
+        <v>0</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="2:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:11" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C17" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="66"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="68"/>
+    </row>
+    <row r="18" spans="2:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" s="64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B19" s="77"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="64"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B20" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="14">
+        <v>8</v>
+      </c>
+      <c r="D20" s="16">
+        <v>8</v>
+      </c>
+      <c r="E20" s="16">
+        <v>0</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="H21" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="G5:N5"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2952,6 +2845,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3095,22 +3003,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3126,21 +3036,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>